<commit_message>
Data updated in excel sheet
</commit_message>
<xml_diff>
--- a/MyStoreProject/src/test/resources/TestData/TestData.xlsx
+++ b/MyStoreProject/src/test/resources/TestData/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10340" windowHeight="3230" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10340" windowHeight="3230" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,6 @@
     <sheet name="AccountCreationData" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:I9"/>
 </workbook>
 </file>
 
@@ -285,16 +284,16 @@
     <t>ABCDEF</t>
   </si>
   <si>
-    <t>newtest1@gmail.com</t>
-  </si>
-  <si>
-    <t>newtest2@gmail.com</t>
-  </si>
-  <si>
-    <t>newtest3@gmail.com</t>
-  </si>
-  <si>
     <t>ahfsdtyfg@gmail.com</t>
+  </si>
+  <si>
+    <t>newtest4@gmail.com</t>
+  </si>
+  <si>
+    <t>newtest5@gmail.com</t>
+  </si>
+  <si>
+    <t>newtest6@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -1067,7 +1066,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -1083,7 +1082,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" s="10" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -1159,8 +1158,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1231,7 +1230,7 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" s="11" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B2" s="12" t="s">
         <v>72</v>
@@ -1278,7 +1277,7 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3" s="11" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B3" s="12" t="s">
         <v>72</v>
@@ -1325,7 +1324,7 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A4" s="11" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B4" s="12" t="s">
         <v>72</v>

</xml_diff>